<commit_message>
Use a Time Interrupt para leer los Pines
</commit_message>
<xml_diff>
--- a/MimicPanel/DriverDesk/DriverDeskTft/PinOut.xlsx
+++ b/MimicPanel/DriverDesk/DriverDeskTft/PinOut.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/daniel/OHS/danielvilas/DigitalTrains/MimicPanel/DriverDesk/DriverDeskTft/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C69A6FBF-8870-5041-A8D9-EBAA5B148814}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C3E68A1-29DB-F84B-8217-0B6A68329A6B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="9760" yWindow="6960" windowWidth="28040" windowHeight="17440" xr2:uid="{7FBBD6A7-D4F6-3247-B6ED-59D4AB52A278}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="61">
   <si>
     <t>STMf103C8T6</t>
   </si>
@@ -190,13 +190,46 @@
   </si>
   <si>
     <t>RENC_S</t>
+  </si>
+  <si>
+    <t>RENC_H</t>
+  </si>
+  <si>
+    <t>BTN_10</t>
+  </si>
+  <si>
+    <t>BTN_9</t>
+  </si>
+  <si>
+    <t>BTN_3</t>
+  </si>
+  <si>
+    <t>BTN_4</t>
+  </si>
+  <si>
+    <t>BTN_5</t>
+  </si>
+  <si>
+    <t>BTN_6</t>
+  </si>
+  <si>
+    <t>BTN_7</t>
+  </si>
+  <si>
+    <t>BTN_8</t>
+  </si>
+  <si>
+    <t>BTN_1</t>
+  </si>
+  <si>
+    <t>BTN_2</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -209,6 +242,12 @@
       <color theme="1"/>
       <name val="Arial"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -576,7 +615,7 @@
   <dimension ref="A1:L18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K29" sqref="K29"/>
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -640,7 +679,7 @@
         <v>11</v>
       </c>
       <c r="D3" t="s">
-        <v>38</v>
+        <v>14</v>
       </c>
       <c r="F3" t="str">
         <f>_xlfn.CONCAT("PB_",A3)</f>
@@ -650,7 +689,7 @@
         <v>14</v>
       </c>
       <c r="H3" t="s">
-        <v>14</v>
+        <v>55</v>
       </c>
       <c r="J3" t="str">
         <f>_xlfn.CONCAT("PC_",A3)</f>
@@ -685,7 +724,7 @@
         <v>14</v>
       </c>
       <c r="H4" t="s">
-        <v>14</v>
+        <v>54</v>
       </c>
       <c r="J4" t="str">
         <f t="shared" ref="J4:J18" si="2">_xlfn.CONCAT("PC_",A4)</f>
@@ -920,7 +959,7 @@
         <v>14</v>
       </c>
       <c r="D11" t="s">
-        <v>14</v>
+        <v>50</v>
       </c>
       <c r="F11" t="str">
         <f t="shared" si="1"/>
@@ -930,7 +969,7 @@
         <v>14</v>
       </c>
       <c r="H11" t="s">
-        <v>14</v>
+        <v>53</v>
       </c>
       <c r="J11" t="str">
         <f t="shared" si="2"/>
@@ -955,7 +994,7 @@
         <v>24</v>
       </c>
       <c r="D12" t="s">
-        <v>14</v>
+        <v>38</v>
       </c>
       <c r="F12" t="str">
         <f t="shared" si="1"/>
@@ -965,7 +1004,7 @@
         <v>14</v>
       </c>
       <c r="H12" t="s">
-        <v>14</v>
+        <v>60</v>
       </c>
       <c r="J12" t="str">
         <f t="shared" si="2"/>
@@ -1000,7 +1039,7 @@
         <v>19</v>
       </c>
       <c r="H13" t="s">
-        <v>14</v>
+        <v>59</v>
       </c>
       <c r="J13" t="str">
         <f t="shared" si="2"/>
@@ -1035,7 +1074,7 @@
         <v>20</v>
       </c>
       <c r="H14" t="s">
-        <v>14</v>
+        <v>51</v>
       </c>
       <c r="J14" t="str">
         <f t="shared" si="2"/>
@@ -1070,7 +1109,7 @@
         <v>14</v>
       </c>
       <c r="H15" t="s">
-        <v>14</v>
+        <v>52</v>
       </c>
       <c r="J15" t="str">
         <f t="shared" si="2"/>
@@ -1105,7 +1144,7 @@
         <v>21</v>
       </c>
       <c r="H16" t="s">
-        <v>14</v>
+        <v>58</v>
       </c>
       <c r="J16" t="str">
         <f t="shared" si="2"/>
@@ -1140,7 +1179,7 @@
         <v>22</v>
       </c>
       <c r="H17" t="s">
-        <v>14</v>
+        <v>57</v>
       </c>
       <c r="J17" t="str">
         <f t="shared" si="2"/>
@@ -1175,7 +1214,7 @@
         <v>23</v>
       </c>
       <c r="H18" t="s">
-        <v>14</v>
+        <v>56</v>
       </c>
       <c r="J18" t="str">
         <f t="shared" si="2"/>
@@ -1189,6 +1228,7 @@
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>

</xml_diff>

<commit_message>
Update Pinout (tested cfg)
</commit_message>
<xml_diff>
--- a/MimicPanel/DriverDesk/DriverDeskTft/PinOut.xlsx
+++ b/MimicPanel/DriverDesk/DriverDeskTft/PinOut.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/daniel/OHS/danielvilas/DigitalTrains/MimicPanel/DriverDesk/DriverDeskTft/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C3E68A1-29DB-F84B-8217-0B6A68329A6B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0922624D-906A-9749-A819-9A538A31223E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="9760" yWindow="6960" windowWidth="28040" windowHeight="17440" xr2:uid="{7FBBD6A7-D4F6-3247-B6ED-59D4AB52A278}"/>
   </bookViews>
@@ -615,7 +615,7 @@
   <dimension ref="A1:L18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+      <selection activeCell="H9" sqref="H9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1074,7 +1074,7 @@
         <v>20</v>
       </c>
       <c r="H14" t="s">
-        <v>51</v>
+        <v>56</v>
       </c>
       <c r="J14" t="str">
         <f t="shared" si="2"/>
@@ -1109,7 +1109,7 @@
         <v>14</v>
       </c>
       <c r="H15" t="s">
-        <v>52</v>
+        <v>57</v>
       </c>
       <c r="J15" t="str">
         <f t="shared" si="2"/>
@@ -1179,7 +1179,7 @@
         <v>22</v>
       </c>
       <c r="H17" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
       <c r="J17" t="str">
         <f t="shared" si="2"/>
@@ -1214,7 +1214,7 @@
         <v>23</v>
       </c>
       <c r="H18" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
       <c r="J18" t="str">
         <f t="shared" si="2"/>

</xml_diff>